<commit_message>
Calibration works still. Updated metadata text file generator to use json. Ready to tag some images with json - so they can be used by a clock.
</commit_message>
<xml_diff>
--- a/example-files/calspreadsheet-Sony-20mm.xlsx
+++ b/example-files/calspreadsheet-Sony-20mm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\nate\code\awim\working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7216D3-384F-455D-B8CA-5C697620D453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34974EC0-9BE0-4F97-BA87-BFD1260C71B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="6345" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -671,12 +671,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1035,7 +1036,7 @@
   <dimension ref="A1:L108"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A21" sqref="A21:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1353,10 +1354,10 @@
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
+      <c r="A15" s="5">
         <v>0</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="5">
         <v>0</v>
       </c>
       <c r="C15" s="1"/>
@@ -1427,10 +1428,10 @@
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A18" s="1">
+      <c r="A18" s="2">
         <v>0</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="2">
         <v>-122.1</v>
       </c>
       <c r="C18" s="1"/>
@@ -1501,10 +1502,10 @@
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A21" s="1">
+      <c r="A21" s="2">
         <v>-220</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="2">
         <v>0</v>
       </c>
       <c r="C21" s="1"/>

</xml_diff>